<commit_message>
app ref data - property area type
</commit_message>
<xml_diff>
--- a/rsa-realty-release/2020/01/doc/App_Ref_Data_V5.xlsx
+++ b/rsa-realty-release/2020/01/doc/App_Ref_Data_V5.xlsx
@@ -11,7 +11,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="250">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="258">
   <si>
     <t>DATA_TYPE</t>
   </si>
@@ -2866,6 +2866,30 @@
   </si>
   <si>
     <t>INSERT INTO APP_REF_DATA (DATA_TYPE, DATA_KEY, DATA_VALUE, GROUP_NAME, SUB_GROUP_NAME, APP_NAME, MODULE_NAME, STATUS_ID, STATUS_TITLE, CREATED_BY, UPDATED_BY) VALUES ('POST_PROPERTY_STATUS', '1', 'Active', 'DEFAULT', '', 'REALTY', 'PROPERTY', '1', 'Active', 'System-User', 'System-User');</t>
+  </si>
+  <si>
+    <t>PROPERTY_AREA_TYPE</t>
+  </si>
+  <si>
+    <t>INSERT INTO APP_REF_DATA (DATA_TYPE, DATA_KEY, DATA_VALUE, GROUP_NAME, SUB_GROUP_NAME, APP_NAME, MODULE_NAME, STATUS_ID, STATUS_TITLE, CREATED_BY, UPDATED_BY) VALUES ('PROPERTY_AREA_TYPE', '-1', 'No Data', 'DEFAULT', '', 'REALTY', 'PROPERTY', '1', 'Active', 'System-User', 'System-User');</t>
+  </si>
+  <si>
+    <t>Carpet</t>
+  </si>
+  <si>
+    <t>INSERT INTO APP_REF_DATA (DATA_TYPE, DATA_KEY, DATA_VALUE, GROUP_NAME, SUB_GROUP_NAME, APP_NAME, MODULE_NAME, STATUS_ID, STATUS_TITLE, CREATED_BY, UPDATED_BY) VALUES ('PROPERTY_AREA_TYPE', '1', 'Carpet', 'DEFAULT', '', 'REALTY', 'PROPERTY', '1', 'Active', 'System-User', 'System-User');</t>
+  </si>
+  <si>
+    <t>Built Up</t>
+  </si>
+  <si>
+    <t>INSERT INTO APP_REF_DATA (DATA_TYPE, DATA_KEY, DATA_VALUE, GROUP_NAME, SUB_GROUP_NAME, APP_NAME, MODULE_NAME, STATUS_ID, STATUS_TITLE, CREATED_BY, UPDATED_BY) VALUES ('PROPERTY_AREA_TYPE', '2', 'Built Up', 'DEFAULT', '', 'REALTY', 'PROPERTY', '1', 'Active', 'System-User', 'System-User');</t>
+  </si>
+  <si>
+    <t>Super Built Up</t>
+  </si>
+  <si>
+    <t>INSERT INTO APP_REF_DATA (DATA_TYPE, DATA_KEY, DATA_VALUE, GROUP_NAME, SUB_GROUP_NAME, APP_NAME, MODULE_NAME, STATUS_ID, STATUS_TITLE, CREATED_BY, UPDATED_BY) VALUES ('PROPERTY_AREA_TYPE', '3', 'Super Built Up', 'DEFAULT', '', 'REALTY', 'PROPERTY', '1', 'Active', 'System-User', 'System-User');</t>
   </si>
 </sst>
 </file>
@@ -4413,7 +4437,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <dimension ref="A1:N113"/>
+  <dimension ref="A1:N117"/>
   <sheetViews>
     <sheetView workbookViewId="0" showGridLines="0" defaultGridColor="1"/>
   </sheetViews>
@@ -8845,6 +8869,162 @@
         <v>249</v>
       </c>
     </row>
+    <row r="114" ht="38.65" customHeight="1">
+      <c r="A114" t="s" s="3">
+        <v>250</v>
+      </c>
+      <c r="B114" s="9">
+        <v>-1</v>
+      </c>
+      <c r="C114" t="s" s="3">
+        <v>53</v>
+      </c>
+      <c r="D114" t="s" s="3">
+        <v>17</v>
+      </c>
+      <c r="E114" s="8"/>
+      <c r="F114" t="s" s="3">
+        <v>18</v>
+      </c>
+      <c r="G114" t="s" s="3">
+        <v>19</v>
+      </c>
+      <c r="H114" s="9">
+        <v>1</v>
+      </c>
+      <c r="I114" t="s" s="3">
+        <v>20</v>
+      </c>
+      <c r="J114" t="s" s="3">
+        <v>21</v>
+      </c>
+      <c r="K114" s="8"/>
+      <c r="L114" t="s" s="3">
+        <v>21</v>
+      </c>
+      <c r="M114" s="8"/>
+      <c r="N114" t="s" s="3">
+        <f>CONCATENATE("INSERT INTO APP_REF_DATA (DATA_TYPE, DATA_KEY, DATA_VALUE, GROUP_NAME, SUB_GROUP_NAME, APP_NAME, MODULE_NAME, STATUS_ID, STATUS_TITLE, CREATED_BY, UPDATED_BY) ","VALUES (","'",A114,"', '",B114,"', '",C114,"', '",D114,"', '",E114,"', '",F114,"', '",G114,"', '",H114,"', '",I114,"', '",J114,"', '",L114,"');")</f>
+        <v>251</v>
+      </c>
+    </row>
+    <row r="115" ht="38.65" customHeight="1">
+      <c r="A115" t="s" s="3">
+        <v>250</v>
+      </c>
+      <c r="B115" s="9">
+        <v>1</v>
+      </c>
+      <c r="C115" t="s" s="3">
+        <v>252</v>
+      </c>
+      <c r="D115" t="s" s="3">
+        <v>17</v>
+      </c>
+      <c r="E115" s="8"/>
+      <c r="F115" t="s" s="3">
+        <v>18</v>
+      </c>
+      <c r="G115" t="s" s="3">
+        <v>19</v>
+      </c>
+      <c r="H115" s="9">
+        <v>1</v>
+      </c>
+      <c r="I115" t="s" s="3">
+        <v>20</v>
+      </c>
+      <c r="J115" t="s" s="3">
+        <v>21</v>
+      </c>
+      <c r="K115" s="8"/>
+      <c r="L115" t="s" s="3">
+        <v>21</v>
+      </c>
+      <c r="M115" s="8"/>
+      <c r="N115" t="s" s="3">
+        <f>CONCATENATE("INSERT INTO APP_REF_DATA (DATA_TYPE, DATA_KEY, DATA_VALUE, GROUP_NAME, SUB_GROUP_NAME, APP_NAME, MODULE_NAME, STATUS_ID, STATUS_TITLE, CREATED_BY, UPDATED_BY) ","VALUES (","'",A115,"', '",B115,"', '",C115,"', '",D115,"', '",E115,"', '",F115,"', '",G115,"', '",H115,"', '",I115,"', '",J115,"', '",L115,"');")</f>
+        <v>253</v>
+      </c>
+    </row>
+    <row r="116" ht="38.65" customHeight="1">
+      <c r="A116" t="s" s="3">
+        <v>250</v>
+      </c>
+      <c r="B116" s="9">
+        <v>2</v>
+      </c>
+      <c r="C116" t="s" s="3">
+        <v>254</v>
+      </c>
+      <c r="D116" t="s" s="3">
+        <v>17</v>
+      </c>
+      <c r="E116" s="8"/>
+      <c r="F116" t="s" s="3">
+        <v>18</v>
+      </c>
+      <c r="G116" t="s" s="3">
+        <v>19</v>
+      </c>
+      <c r="H116" s="9">
+        <v>1</v>
+      </c>
+      <c r="I116" t="s" s="3">
+        <v>20</v>
+      </c>
+      <c r="J116" t="s" s="3">
+        <v>21</v>
+      </c>
+      <c r="K116" s="8"/>
+      <c r="L116" t="s" s="3">
+        <v>21</v>
+      </c>
+      <c r="M116" s="8"/>
+      <c r="N116" t="s" s="3">
+        <f>CONCATENATE("INSERT INTO APP_REF_DATA (DATA_TYPE, DATA_KEY, DATA_VALUE, GROUP_NAME, SUB_GROUP_NAME, APP_NAME, MODULE_NAME, STATUS_ID, STATUS_TITLE, CREATED_BY, UPDATED_BY) ","VALUES (","'",A116,"', '",B116,"', '",C116,"', '",D116,"', '",E116,"', '",F116,"', '",G116,"', '",H116,"', '",I116,"', '",J116,"', '",L116,"');")</f>
+        <v>255</v>
+      </c>
+    </row>
+    <row r="117" ht="38.65" customHeight="1">
+      <c r="A117" t="s" s="3">
+        <v>250</v>
+      </c>
+      <c r="B117" s="9">
+        <v>3</v>
+      </c>
+      <c r="C117" t="s" s="3">
+        <v>256</v>
+      </c>
+      <c r="D117" t="s" s="3">
+        <v>17</v>
+      </c>
+      <c r="E117" s="8"/>
+      <c r="F117" t="s" s="3">
+        <v>18</v>
+      </c>
+      <c r="G117" t="s" s="3">
+        <v>19</v>
+      </c>
+      <c r="H117" s="9">
+        <v>1</v>
+      </c>
+      <c r="I117" t="s" s="3">
+        <v>20</v>
+      </c>
+      <c r="J117" t="s" s="3">
+        <v>21</v>
+      </c>
+      <c r="K117" s="8"/>
+      <c r="L117" t="s" s="3">
+        <v>21</v>
+      </c>
+      <c r="M117" s="8"/>
+      <c r="N117" t="s" s="3">
+        <f>CONCATENATE("INSERT INTO APP_REF_DATA (DATA_TYPE, DATA_KEY, DATA_VALUE, GROUP_NAME, SUB_GROUP_NAME, APP_NAME, MODULE_NAME, STATUS_ID, STATUS_TITLE, CREATED_BY, UPDATED_BY) ","VALUES (","'",A117,"', '",B117,"', '",C117,"', '",D117,"', '",E117,"', '",F117,"', '",G117,"', '",H117,"', '",I117,"', '",J117,"', '",L117,"');")</f>
+        <v>257</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup firstPageNumber="1" fitToHeight="1" fitToWidth="1" scale="100" useFirstPageNumber="0" orientation="portrait" pageOrder="downThenOver"/>

</xml_diff>